<commit_message>
change time window for sleep - 6AM to 6AM
</commit_message>
<xml_diff>
--- a/raw_data/diapers.xlsx
+++ b/raw_data/diapers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coons/Projects/stink_bean/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491DC4F2-F565-3448-A3C8-6F0CED3ED650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A50C078-5272-3944-95A9-1A4C270F301D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="2060" windowWidth="11860" windowHeight="16940" xr2:uid="{42AB8D47-1E0D-C348-AA78-3B31B749EE61}"/>
+    <workbookView xWindow="9620" yWindow="800" windowWidth="11860" windowHeight="16940" xr2:uid="{42AB8D47-1E0D-C348-AA78-3B31B749EE61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>PM</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{824E54FF-0E43-8F4B-AA4E-86E123E067B4}">
-  <dimension ref="A1:E1317"/>
+  <dimension ref="A1:E1472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1290" workbookViewId="0">
-      <selection activeCell="E1312" sqref="E1312:E1317"/>
+    <sheetView tabSelected="1" topLeftCell="A1438" workbookViewId="0">
+      <selection activeCell="E1465" sqref="E1465:E1472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22808,6 +22811,2641 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1318" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1318" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B1318" s="1">
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="C1318" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1318">
+        <v>0</v>
+      </c>
+      <c r="E1318">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1319" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B1319" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C1319" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1319">
+        <v>0</v>
+      </c>
+      <c r="E1319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1320" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B1320" s="1">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="C1320" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1320">
+        <v>0</v>
+      </c>
+      <c r="E1320">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1321" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B1321" s="1">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C1321" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1321">
+        <v>1</v>
+      </c>
+      <c r="E1321">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1322" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B1322" s="1">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="C1322" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1322">
+        <v>0</v>
+      </c>
+      <c r="E1322">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1323" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B1323" s="1">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="C1323" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1323">
+        <v>0</v>
+      </c>
+      <c r="E1323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1324" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B1324" s="1">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="C1324" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1324">
+        <v>0</v>
+      </c>
+      <c r="E1324">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1325" s="2">
+        <v>43922</v>
+      </c>
+      <c r="B1325" s="1">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="C1325" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1325">
+        <v>0</v>
+      </c>
+      <c r="E1325">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1326" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B1326" s="1">
+        <v>0.22708333333333333</v>
+      </c>
+      <c r="C1326" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1326">
+        <v>0</v>
+      </c>
+      <c r="E1326">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1327" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B1327" s="1">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C1327" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1327">
+        <v>0</v>
+      </c>
+      <c r="E1327">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1328" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B1328" s="1">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="C1328" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1328">
+        <v>0</v>
+      </c>
+      <c r="E1328">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1329" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B1329" s="1">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="C1329" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1329">
+        <v>0</v>
+      </c>
+      <c r="E1329">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1330" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B1330" s="1">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="C1330" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1330">
+        <v>0</v>
+      </c>
+      <c r="E1330">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1331" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B1331" s="1">
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="C1331" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1331">
+        <v>1</v>
+      </c>
+      <c r="E1331">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1332" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B1332" s="1">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="C1332" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1332">
+        <v>1</v>
+      </c>
+      <c r="E1332">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1333" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B1333" s="1">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="C1333" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1333">
+        <v>1</v>
+      </c>
+      <c r="E1333">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1334" s="2">
+        <v>43923</v>
+      </c>
+      <c r="B1334" s="1">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C1334" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1334">
+        <v>0</v>
+      </c>
+      <c r="E1334">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1335" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B1335" s="1">
+        <v>0.18541666666666667</v>
+      </c>
+      <c r="C1335" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1335">
+        <v>0</v>
+      </c>
+      <c r="E1335">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1336" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B1336" s="1">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="C1336" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1336">
+        <v>1</v>
+      </c>
+      <c r="E1336">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1337" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B1337" s="1">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="C1337" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1337">
+        <v>0</v>
+      </c>
+      <c r="E1337">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1338" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B1338" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C1338" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1338">
+        <v>0</v>
+      </c>
+      <c r="E1338">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1339" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B1339" s="1">
+        <v>0.15069444444444444</v>
+      </c>
+      <c r="C1339" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1339">
+        <v>0</v>
+      </c>
+      <c r="E1339">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1340" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B1340" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C1340" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1340">
+        <v>0</v>
+      </c>
+      <c r="E1340">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1341" s="2">
+        <v>43924</v>
+      </c>
+      <c r="B1341" s="1">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="C1341" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1341">
+        <v>0</v>
+      </c>
+      <c r="E1341">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1342" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B1342" s="1">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="C1342" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1342">
+        <v>0</v>
+      </c>
+      <c r="E1342">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1343" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B1343" s="1">
+        <v>0.21319444444444444</v>
+      </c>
+      <c r="C1343" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1343">
+        <v>1</v>
+      </c>
+      <c r="E1343">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1344" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B1344" s="1">
+        <v>0.28125</v>
+      </c>
+      <c r="C1344" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1344">
+        <v>0</v>
+      </c>
+      <c r="E1344">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1345" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B1345" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="C1345" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1345">
+        <v>0</v>
+      </c>
+      <c r="E1345">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1346" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B1346" s="1">
+        <v>0.48472222222222222</v>
+      </c>
+      <c r="C1346" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1346">
+        <v>0</v>
+      </c>
+      <c r="E1346">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1347" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B1347" s="1">
+        <v>0.5229166666666667</v>
+      </c>
+      <c r="C1347" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1347">
+        <v>0</v>
+      </c>
+      <c r="E1347">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1348" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B1348" s="1">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="C1348" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1348">
+        <v>0</v>
+      </c>
+      <c r="E1348">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1349" s="2">
+        <v>43925</v>
+      </c>
+      <c r="B1349" s="1">
+        <v>0.27708333333333335</v>
+      </c>
+      <c r="C1349" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1349">
+        <v>1</v>
+      </c>
+      <c r="E1349">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1350" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B1350" s="1">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="C1350" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1350">
+        <v>0</v>
+      </c>
+      <c r="E1350">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1351" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B1351" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="C1351" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1351">
+        <v>0</v>
+      </c>
+      <c r="E1351">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1352" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B1352" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C1352" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1352">
+        <v>1</v>
+      </c>
+      <c r="E1352">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1353" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B1353" s="1">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C1353" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1353">
+        <v>0</v>
+      </c>
+      <c r="E1353">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1354" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B1354" s="1">
+        <v>0.52916666666666667</v>
+      </c>
+      <c r="C1354" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1354">
+        <v>0</v>
+      </c>
+      <c r="E1354">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1355" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B1355" s="1">
+        <v>0.14652777777777778</v>
+      </c>
+      <c r="C1355" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1355">
+        <v>1</v>
+      </c>
+      <c r="E1355">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1356" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B1356" s="1">
+        <v>0.3125</v>
+      </c>
+      <c r="C1356" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1356">
+        <v>0</v>
+      </c>
+      <c r="E1356">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1357" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B1357" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C1357" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1357">
+        <v>0</v>
+      </c>
+      <c r="E1357">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1358" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B1358" s="1">
+        <v>0.29097222222222224</v>
+      </c>
+      <c r="C1358" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1358">
+        <v>0</v>
+      </c>
+      <c r="E1358">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1359" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B1359" s="1">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C1359" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1359">
+        <v>1</v>
+      </c>
+      <c r="E1359">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1360" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B1360" s="1">
+        <v>0.49027777777777781</v>
+      </c>
+      <c r="C1360" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1360">
+        <v>0</v>
+      </c>
+      <c r="E1360">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1361" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B1361" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C1361" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1361">
+        <v>0</v>
+      </c>
+      <c r="E1361">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1362" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B1362" s="1">
+        <v>0.22569444444444445</v>
+      </c>
+      <c r="C1362" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1362">
+        <v>1</v>
+      </c>
+      <c r="E1362">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1363" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B1363" s="1">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C1363" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1363">
+        <v>0</v>
+      </c>
+      <c r="E1363">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1364" s="2">
+        <v>43928</v>
+      </c>
+      <c r="B1364" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C1364" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1364">
+        <v>0</v>
+      </c>
+      <c r="E1364">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1365" s="2">
+        <v>43928</v>
+      </c>
+      <c r="B1365" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C1365" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1365">
+        <v>0</v>
+      </c>
+      <c r="E1365">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1366" s="2">
+        <v>43928</v>
+      </c>
+      <c r="B1366" s="1">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C1366" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1366">
+        <v>0</v>
+      </c>
+      <c r="E1366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1367" s="2">
+        <v>43928</v>
+      </c>
+      <c r="B1367" s="1">
+        <v>0.4770833333333333</v>
+      </c>
+      <c r="C1367" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1367">
+        <v>1</v>
+      </c>
+      <c r="E1367">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1368" s="2">
+        <v>43928</v>
+      </c>
+      <c r="B1368" s="1">
+        <v>0.12152777777777778</v>
+      </c>
+      <c r="C1368" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1368">
+        <v>0</v>
+      </c>
+      <c r="E1368">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1369" s="2">
+        <v>43928</v>
+      </c>
+      <c r="B1369" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C1369" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1369">
+        <v>1</v>
+      </c>
+      <c r="E1369">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1370" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B1370" s="1">
+        <v>0.13958333333333334</v>
+      </c>
+      <c r="C1370" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1370">
+        <v>0</v>
+      </c>
+      <c r="E1370">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1371" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B1371" s="1">
+        <v>0.31736111111111115</v>
+      </c>
+      <c r="C1371" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1371">
+        <v>0</v>
+      </c>
+      <c r="E1371">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1372" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B1372" s="1">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C1372" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1372">
+        <v>0</v>
+      </c>
+      <c r="E1372">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1373" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B1373" s="1">
+        <v>0.50972222222222219</v>
+      </c>
+      <c r="C1373" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1373">
+        <v>0</v>
+      </c>
+      <c r="E1373">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1374" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B1374" s="1">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="C1374" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1374">
+        <v>0</v>
+      </c>
+      <c r="E1374">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1375" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B1375" s="1">
+        <v>0.23611111111111113</v>
+      </c>
+      <c r="C1375" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1375">
+        <v>1</v>
+      </c>
+      <c r="E1375">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1376" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B1376" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C1376" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1376">
+        <v>0</v>
+      </c>
+      <c r="E1376">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1377" s="2">
+        <v>43930</v>
+      </c>
+      <c r="B1377" s="1">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="C1377" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1377">
+        <v>1</v>
+      </c>
+      <c r="E1377">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1378" s="2">
+        <v>43930</v>
+      </c>
+      <c r="B1378" s="1">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="C1378" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1378">
+        <v>0</v>
+      </c>
+      <c r="E1378">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1379" s="2">
+        <v>43930</v>
+      </c>
+      <c r="B1379" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C1379" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1379">
+        <v>0</v>
+      </c>
+      <c r="E1379">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1380" s="2">
+        <v>43930</v>
+      </c>
+      <c r="B1380" s="1">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C1380" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1380">
+        <v>0</v>
+      </c>
+      <c r="E1380">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1381" s="2">
+        <v>43930</v>
+      </c>
+      <c r="B1381" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C1381" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1381">
+        <v>0</v>
+      </c>
+      <c r="E1381">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1382" s="2">
+        <v>43930</v>
+      </c>
+      <c r="B1382" s="1">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="C1382" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1382">
+        <v>0</v>
+      </c>
+      <c r="E1382">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1383" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B1383" s="1">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="C1383" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1383">
+        <v>0</v>
+      </c>
+      <c r="E1383">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1384" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B1384" s="1">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="C1384" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1384">
+        <v>1</v>
+      </c>
+      <c r="E1384">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1385" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B1385" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C1385" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1385">
+        <v>0</v>
+      </c>
+      <c r="E1385">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1386" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B1386" s="1">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="C1386" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1386">
+        <v>1</v>
+      </c>
+      <c r="E1386">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1387" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B1387" s="1">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="C1387" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1387">
+        <v>1</v>
+      </c>
+      <c r="E1387">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1388" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B1388" s="1">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="C1388" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1388">
+        <v>0</v>
+      </c>
+      <c r="E1388">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1389" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B1389" s="1">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="C1389" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1389">
+        <v>0</v>
+      </c>
+      <c r="E1389">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1390" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B1390" s="1">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="C1390" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1390">
+        <v>0</v>
+      </c>
+      <c r="E1390">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1391" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B1391" s="1">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="C1391" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1391">
+        <v>0</v>
+      </c>
+      <c r="E1391">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1392" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B1392" s="1">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="C1392" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1392">
+        <v>0</v>
+      </c>
+      <c r="E1392">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1393" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B1393" s="1">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C1393" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1393">
+        <v>0</v>
+      </c>
+      <c r="E1393">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1394" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B1394" s="1">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="C1394" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1394">
+        <v>1</v>
+      </c>
+      <c r="E1394">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1395" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B1395" s="1">
+        <v>0.11805555555555557</v>
+      </c>
+      <c r="C1395" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1395">
+        <v>0</v>
+      </c>
+      <c r="E1395">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1396" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B1396" s="1">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C1396" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1396">
+        <v>0</v>
+      </c>
+      <c r="E1396">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1397" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B1397" s="1">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="C1397" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1397">
+        <v>0</v>
+      </c>
+      <c r="E1397">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1398" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B1398" s="1">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="C1398" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1398">
+        <v>1</v>
+      </c>
+      <c r="E1398">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1399" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B1399" s="1">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="C1399" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1399">
+        <v>0</v>
+      </c>
+      <c r="E1399">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1400" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B1400" s="1">
+        <v>0.48680555555555555</v>
+      </c>
+      <c r="C1400" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1400">
+        <v>0</v>
+      </c>
+      <c r="E1400">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1401" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B1401" s="1">
+        <v>0.11805555555555557</v>
+      </c>
+      <c r="C1401" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1401">
+        <v>0</v>
+      </c>
+      <c r="E1401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1402" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B1402" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C1402" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1402">
+        <v>0</v>
+      </c>
+      <c r="E1402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1403" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B1403" s="1">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="C1403" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1403">
+        <v>0</v>
+      </c>
+      <c r="E1403">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1404" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B1404" s="1">
+        <v>0.10069444444444443</v>
+      </c>
+      <c r="C1404" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1404">
+        <v>0</v>
+      </c>
+      <c r="E1404">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1405" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B1405" s="1">
+        <v>0.27847222222222223</v>
+      </c>
+      <c r="C1405" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1405">
+        <v>1</v>
+      </c>
+      <c r="E1405">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1406" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B1406" s="1">
+        <v>0.35902777777777778</v>
+      </c>
+      <c r="C1406" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1406">
+        <v>0</v>
+      </c>
+      <c r="E1406">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1407" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B1407" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="C1407" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1407">
+        <v>0</v>
+      </c>
+      <c r="E1407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1408" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B1408" s="1">
+        <v>8.1944444444444445E-2</v>
+      </c>
+      <c r="C1408" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1408">
+        <v>0</v>
+      </c>
+      <c r="E1408">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1409" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B1409" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C1409" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1409">
+        <v>0</v>
+      </c>
+      <c r="E1409">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1410" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B1410" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C1410" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1410">
+        <v>0</v>
+      </c>
+      <c r="E1410">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1411" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B1411" s="1">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="C1411" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1411">
+        <v>0</v>
+      </c>
+      <c r="E1411">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1412" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B1412" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C1412" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1412">
+        <v>0</v>
+      </c>
+      <c r="E1412">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1413" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B1413" s="1">
+        <v>0.42152777777777778</v>
+      </c>
+      <c r="C1413" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1413">
+        <v>0</v>
+      </c>
+      <c r="E1413">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1414" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B1414" s="1">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="C1414" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1414">
+        <v>1</v>
+      </c>
+      <c r="E1414">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1415" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B1415" s="1">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C1415" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1415">
+        <v>0</v>
+      </c>
+      <c r="E1415">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1416" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B1416" s="1">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="C1416" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1416">
+        <v>0</v>
+      </c>
+      <c r="E1416">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1417" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B1417" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C1417" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1417">
+        <v>0</v>
+      </c>
+      <c r="E1417">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1418" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B1418" s="1">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="C1418" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1418">
+        <v>1</v>
+      </c>
+      <c r="E1418">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1419" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B1419" s="1">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="C1419" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1419">
+        <v>0</v>
+      </c>
+      <c r="E1419">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1420" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B1420" s="1">
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="C1420" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1420">
+        <v>0</v>
+      </c>
+      <c r="E1420">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1421" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B1421" s="1">
+        <v>0.3520833333333333</v>
+      </c>
+      <c r="C1421" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1421">
+        <v>0</v>
+      </c>
+      <c r="E1421">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1422" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B1422" s="1">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="C1422" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1422">
+        <v>0</v>
+      </c>
+      <c r="E1422">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1423" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B1423" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C1423" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1423">
+        <v>1</v>
+      </c>
+      <c r="E1423">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1424" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B1424" s="1">
+        <v>0.11319444444444444</v>
+      </c>
+      <c r="C1424" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1424">
+        <v>0</v>
+      </c>
+      <c r="E1424">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1425" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B1425" s="1">
+        <v>0.2673611111111111</v>
+      </c>
+      <c r="C1425" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1425">
+        <v>0</v>
+      </c>
+      <c r="E1425">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1426" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B1426" s="1">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="C1426" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1426">
+        <v>0</v>
+      </c>
+      <c r="E1426">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1427" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B1427" s="1">
+        <v>0.29583333333333334</v>
+      </c>
+      <c r="C1427" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1427">
+        <v>1</v>
+      </c>
+      <c r="E1427">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1428" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B1428" s="1">
+        <v>0.41041666666666665</v>
+      </c>
+      <c r="C1428" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1428">
+        <v>0</v>
+      </c>
+      <c r="E1428">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1429" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B1429" s="1">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="C1429" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1429">
+        <v>1</v>
+      </c>
+      <c r="E1429">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1430" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B1430" s="1">
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="C1430" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1430">
+        <v>0</v>
+      </c>
+      <c r="E1430">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1431" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B1431" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C1431" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1431">
+        <v>1</v>
+      </c>
+      <c r="E1431">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1432" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B1432" s="1">
+        <v>0.30763888888888891</v>
+      </c>
+      <c r="C1432" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1432">
+        <v>0</v>
+      </c>
+      <c r="E1432">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1433" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B1433" s="1">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C1433" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1433">
+        <v>0</v>
+      </c>
+      <c r="E1433">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1434" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B1434" s="1">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C1434" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1434">
+        <v>1</v>
+      </c>
+      <c r="E1434">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1435" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B1435" s="1">
+        <v>0.30833333333333335</v>
+      </c>
+      <c r="C1435" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1435">
+        <v>0</v>
+      </c>
+      <c r="E1435">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1436" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B1436" s="1">
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="C1436" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1436">
+        <v>0</v>
+      </c>
+      <c r="E1436">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1437" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B1437" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C1437" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1437">
+        <v>0</v>
+      </c>
+      <c r="E1437">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1438" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B1438" s="1">
+        <v>0.19305555555555554</v>
+      </c>
+      <c r="C1438" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1438">
+        <v>0</v>
+      </c>
+      <c r="E1438">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1439" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B1439" s="1">
+        <v>0.30763888888888891</v>
+      </c>
+      <c r="C1439" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1439">
+        <v>0</v>
+      </c>
+      <c r="E1439">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1440" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B1440" s="1">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="C1440" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1440">
+        <v>0</v>
+      </c>
+      <c r="E1440">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1441" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B1441" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C1441" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1441">
+        <v>0</v>
+      </c>
+      <c r="E1441">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1442" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B1442" s="1">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="C1442" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1442">
+        <v>0</v>
+      </c>
+      <c r="E1442">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1443" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B1443" s="1">
+        <v>0.37291666666666662</v>
+      </c>
+      <c r="C1443" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1443">
+        <v>1</v>
+      </c>
+      <c r="E1443">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1444" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B1444" s="1">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="C1444" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1444">
+        <v>0</v>
+      </c>
+      <c r="E1444">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1445" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B1445" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C1445" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1445">
+        <v>0</v>
+      </c>
+      <c r="E1445">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1446" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B1446" s="1">
+        <v>0.19791666666666666</v>
+      </c>
+      <c r="C1446" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1446">
+        <v>0</v>
+      </c>
+      <c r="E1446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1447" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B1447" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C1447" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1447">
+        <v>0</v>
+      </c>
+      <c r="E1447">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1448" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B1448" s="1">
+        <v>0.29583333333333334</v>
+      </c>
+      <c r="C1448" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1448">
+        <v>1</v>
+      </c>
+      <c r="E1448">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1449" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B1449" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="C1449" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1449">
+        <v>0</v>
+      </c>
+      <c r="E1449">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1450" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B1450" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C1450" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1450">
+        <v>0</v>
+      </c>
+      <c r="E1450">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1451" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B1451" s="1">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C1451" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1451">
+        <v>0</v>
+      </c>
+      <c r="E1451">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1452" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B1452" s="1">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="C1452" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1452">
+        <v>1</v>
+      </c>
+      <c r="E1452">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1453" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B1453" s="1">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="C1453" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1453">
+        <v>0</v>
+      </c>
+      <c r="E1453">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1454" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B1454" s="1">
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="C1454" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1454">
+        <v>0</v>
+      </c>
+      <c r="E1454">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1455" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B1455" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C1455" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1455">
+        <v>1</v>
+      </c>
+      <c r="E1455">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1456" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B1456" s="1">
+        <v>0.22569444444444445</v>
+      </c>
+      <c r="C1456" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1456">
+        <v>0</v>
+      </c>
+      <c r="E1456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1457" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B1457" s="1">
+        <v>0.30138888888888887</v>
+      </c>
+      <c r="C1457" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1457">
+        <v>0</v>
+      </c>
+      <c r="E1457">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1458" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B1458" s="1">
+        <v>0.34583333333333338</v>
+      </c>
+      <c r="C1458" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1458">
+        <v>0</v>
+      </c>
+      <c r="E1458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1459" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B1459" s="1">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="C1459" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1459">
+        <v>0</v>
+      </c>
+      <c r="E1459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1460" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B1460" s="1">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="C1460" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1460">
+        <v>1</v>
+      </c>
+      <c r="E1460">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1461" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B1461" s="1">
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="C1461" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1461">
+        <v>1</v>
+      </c>
+      <c r="E1461">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1462" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B1462" s="1">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C1462" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1462">
+        <v>0</v>
+      </c>
+      <c r="E1462">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1463" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B1463" s="1">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C1463" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1463">
+        <v>0</v>
+      </c>
+      <c r="E1463">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1464" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B1464" s="1">
+        <v>0.25694444444444448</v>
+      </c>
+      <c r="C1464" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1464">
+        <v>0</v>
+      </c>
+      <c r="E1464">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1465" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B1465" s="1">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C1465" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1465">
+        <v>0</v>
+      </c>
+      <c r="E1465" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1466" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B1466" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C1466" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1466">
+        <v>0</v>
+      </c>
+      <c r="E1466">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1467" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B1467" s="1">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="C1467" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1467">
+        <v>0</v>
+      </c>
+      <c r="E1467">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1468" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B1468" s="1">
+        <v>0.1763888888888889</v>
+      </c>
+      <c r="C1468" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1468">
+        <v>0</v>
+      </c>
+      <c r="E1468">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1469" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B1469" s="1">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="C1469" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1469">
+        <v>0</v>
+      </c>
+      <c r="E1469">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1470" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B1470" s="1">
+        <v>0.15625</v>
+      </c>
+      <c r="C1470" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1470">
+        <v>0</v>
+      </c>
+      <c r="E1470">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1471" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B1471" s="1">
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="C1471" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1471">
+        <v>1</v>
+      </c>
+      <c r="E1471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1472" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B1472" s="1">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="C1472" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1472">
+        <v>0</v>
+      </c>
+      <c r="E1472">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>